<commit_message>
Improvements and bug fixes to outlier_all_stats; but still something is wrong
</commit_message>
<xml_diff>
--- a/tables/fixed_outlier_rates.xlsx
+++ b/tables/fixed_outlier_rates.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="fixed_outlier_rates" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="24">
   <si>
     <t>AGO_IND</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>WATER</t>
+  </si>
+  <si>
+    <t>MIN_FIXED2</t>
+  </si>
+  <si>
+    <t>MAX_FIXED2</t>
   </si>
 </sst>
 </file>
@@ -568,8 +574,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -891,11 +898,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,12 +910,15 @@
     <col min="1" max="2" width="5.140625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -921,13 +931,13 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -939,8 +949,26 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -953,13 +981,13 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>30</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>40</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>150</v>
       </c>
       <c r="H2">
@@ -971,8 +999,26 @@
       <c r="J2">
         <v>2.1800000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="1">
+        <v>6.8443708450083195E-11</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -985,13 +1031,13 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>200</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>300</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>3000</v>
       </c>
       <c r="H3">
@@ -1003,8 +1049,26 @@
       <c r="J3">
         <v>3.48</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="1">
+        <v>3.2266319697896301E-9</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1017,13 +1081,13 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>2000</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>3000</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>4000</v>
       </c>
       <c r="H4">
@@ -1035,8 +1099,26 @@
       <c r="J4">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1.2935860897065699E-6</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>3018.1086519114601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1049,13 +1131,13 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>30</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>40</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>150</v>
       </c>
       <c r="H5">
@@ -1067,8 +1149,26 @@
       <c r="J5">
         <v>2.1800000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="1">
+        <v>1.6209751617927999E-8</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1081,13 +1181,13 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0.2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>5</v>
       </c>
       <c r="H6">
@@ -1099,8 +1199,26 @@
       <c r="J6">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" s="1">
+        <v>3.24675324675324E-3</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>2360824.7422680398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1113,13 +1231,13 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>0.2</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>5</v>
       </c>
       <c r="H7">
@@ -1131,8 +1249,26 @@
       <c r="J7">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" t="s">
+        <v>12</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.76893939393939303</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1238095.23809523</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1145,13 +1281,13 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>10</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1">
         <v>50</v>
       </c>
       <c r="H8">
@@ -1163,8 +1299,26 @@
       <c r="J8">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1177,13 +1331,13 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9">
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
         <v>50</v>
       </c>
       <c r="H9">
@@ -1195,8 +1349,26 @@
       <c r="J9">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O9" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="1">
+        <v>7.6893939393939297</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1209,13 +1381,13 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>20</v>
-      </c>
-      <c r="G10">
+      <c r="E10" s="1">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1">
         <v>50</v>
       </c>
       <c r="H10">
@@ -1227,8 +1399,26 @@
       <c r="J10">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="1">
+        <v>6.4935064935064901E-2</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>41.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1241,13 +1431,13 @@
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>100</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>300</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>500</v>
       </c>
       <c r="H11">
@@ -1259,8 +1449,26 @@
       <c r="J11">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" s="1">
+        <v>6.6225165562913899</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>397.67441860465101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1273,13 +1481,13 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>20</v>
-      </c>
-      <c r="G12">
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1">
         <v>50</v>
       </c>
       <c r="H12">
@@ -1291,8 +1499,26 @@
       <c r="J12">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="1">
+        <v>15.378787878787801</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>23.446153846153798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1305,13 +1531,13 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>130</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>300</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>10000</v>
       </c>
       <c r="H13">
@@ -1323,8 +1549,26 @@
       <c r="J13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" s="1">
+        <v>1.0600134847166899E-10</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>708.247422680412</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1337,13 +1581,13 @@
       <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>3000</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>10000</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>50000</v>
       </c>
       <c r="H14">
@@ -1355,8 +1599,26 @@
       <c r="J14">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" s="1">
+        <v>1.19092052703144E-7</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1369,13 +1631,13 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>3000</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>10000</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>50000</v>
       </c>
       <c r="H15">
@@ -1387,8 +1649,26 @@
       <c r="J15">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O15" t="s">
+        <v>20</v>
+      </c>
+      <c r="P15" s="1">
+        <v>8.3213140273522205E-9</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1401,13 +1681,13 @@
       <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>100</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>300</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>3000</v>
       </c>
       <c r="H16">
@@ -1419,8 +1699,26 @@
       <c r="J16">
         <v>3.48</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" t="s">
+        <v>15</v>
+      </c>
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P16" s="1">
+        <v>1.15037173639728E-7</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>371.42857142857099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1433,13 +1731,13 @@
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>10000</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>30000</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>50000</v>
       </c>
       <c r="H17">
@@ -1451,8 +1749,26 @@
       <c r="J17">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" t="s">
+        <v>16</v>
+      </c>
+      <c r="N17" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" t="s">
+        <v>20</v>
+      </c>
+      <c r="P17" s="1">
+        <v>6.7044920096464594E-2</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>810000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1465,13 +1781,13 @@
       <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>30000</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>40000</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>50000</v>
       </c>
       <c r="H18">
@@ -1483,8 +1799,26 @@
       <c r="J18">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" t="s">
+        <v>16</v>
+      </c>
+      <c r="N18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O18" t="s">
+        <v>20</v>
+      </c>
+      <c r="P18" s="1">
+        <v>72.760000000000005</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>105000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1497,13 +1831,13 @@
       <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>30000</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>40000</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>50000</v>
       </c>
       <c r="H19">
@@ -1515,8 +1849,26 @@
       <c r="J19">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" t="s">
+        <v>20</v>
+      </c>
+      <c r="P19" s="1">
+        <v>1.3408984019292901E-3</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>484150000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1529,13 +1881,13 @@
       <c r="D20" t="s">
         <v>21</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>10000</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>30000</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>50000</v>
       </c>
       <c r="H20">
@@ -1547,8 +1899,26 @@
       <c r="J20">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" t="s">
+        <v>17</v>
+      </c>
+      <c r="N20" t="s">
+        <v>13</v>
+      </c>
+      <c r="O20" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1561,13 +1931,13 @@
       <c r="D21" t="s">
         <v>20</v>
       </c>
-      <c r="E21">
-        <v>20</v>
-      </c>
-      <c r="F21">
+      <c r="E21" s="1">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1">
         <v>100</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>200</v>
       </c>
       <c r="H21">
@@ -1579,8 +1949,26 @@
       <c r="J21">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" t="s">
+        <v>17</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" t="s">
+        <v>20</v>
+      </c>
+      <c r="P21" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>200000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1593,13 +1981,13 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="E22">
-        <v>20</v>
-      </c>
-      <c r="F22">
+      <c r="E22" s="1">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1">
         <v>100</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>200</v>
       </c>
       <c r="H22">
@@ -1611,8 +1999,26 @@
       <c r="J22">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O22" t="s">
+        <v>20</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1.4552</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1625,13 +2031,13 @@
       <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>1000</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>3000</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>5000</v>
       </c>
       <c r="H23">
@@ -1643,8 +2049,26 @@
       <c r="J23">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" t="s">
+        <v>20</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0.670449200964646</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1657,13 +2081,13 @@
       <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>1000</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>3000</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>5000</v>
       </c>
       <c r="H24">
@@ -1675,8 +2099,26 @@
       <c r="J24">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" t="s">
+        <v>13</v>
+      </c>
+      <c r="O24" t="s">
+        <v>20</v>
+      </c>
+      <c r="P24" s="1">
+        <v>48.753894080996801</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1689,13 +2131,13 @@
       <c r="D25" t="s">
         <v>20</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>2</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>10</v>
       </c>
       <c r="H25">
@@ -1707,8 +2149,26 @@
       <c r="J25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" t="s">
+        <v>18</v>
+      </c>
+      <c r="N25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" t="s">
+        <v>20</v>
+      </c>
+      <c r="P25" s="1">
+        <v>41.6666666666666</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1721,13 +2181,13 @@
       <c r="D26" t="s">
         <v>20</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>5</v>
       </c>
-      <c r="F26">
-        <v>10</v>
-      </c>
-      <c r="G26">
+      <c r="F26" s="1">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1">
         <v>20</v>
       </c>
       <c r="H26">
@@ -1739,8 +2199,26 @@
       <c r="J26">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" t="s">
+        <v>20</v>
+      </c>
+      <c r="P26" s="1">
+        <v>727.6</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -1753,13 +2231,13 @@
       <c r="D27" t="s">
         <v>20</v>
       </c>
-      <c r="E27">
-        <v>10</v>
-      </c>
-      <c r="F27">
+      <c r="E27" s="1">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1">
         <v>50</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>100</v>
       </c>
       <c r="H27">
@@ -1772,7 +2250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1785,13 +2263,13 @@
       <c r="D28" t="s">
         <v>20</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>1</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>2</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>10</v>
       </c>
       <c r="H28">
@@ -1804,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1817,13 +2295,13 @@
       <c r="D29" t="s">
         <v>21</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>100</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>500</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <v>1000</v>
       </c>
       <c r="H29">
@@ -1836,7 +2314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1849,13 +2327,13 @@
       <c r="D30" t="s">
         <v>21</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>100</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>500</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>1000</v>
       </c>
       <c r="H30">
@@ -1868,7 +2346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1881,13 +2359,13 @@
       <c r="D31" t="s">
         <v>20</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>500</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>1000</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <v>5000</v>
       </c>
       <c r="H31">
@@ -1900,7 +2378,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1913,13 +2391,13 @@
       <c r="D32" t="s">
         <v>20</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>500</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>1000</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>5000</v>
       </c>
       <c r="H32">
@@ -1945,13 +2423,13 @@
       <c r="D33" t="s">
         <v>20</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>5000</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>8000</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>20000</v>
       </c>
       <c r="H33">
@@ -1977,13 +2455,13 @@
       <c r="D34" t="s">
         <v>20</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>500</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>1000</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>5000</v>
       </c>
       <c r="H34">
@@ -2009,13 +2487,13 @@
       <c r="D35" t="s">
         <v>21</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>5000</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>80000</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>100000</v>
       </c>
       <c r="H35">
@@ -2041,13 +2519,13 @@
       <c r="D36" t="s">
         <v>21</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>5000</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>80000</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>100000</v>
       </c>
       <c r="H36">
@@ -2061,6 +2539,11 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="L2:Q26">
+    <sortCondition ref="L2:L26"/>
+    <sortCondition ref="M2:M26"/>
+    <sortCondition descending="1" ref="N2:N26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>